<commit_message>
full restructure created - Problem :excel file overwrites data
</commit_message>
<xml_diff>
--- a/tweet.xlsx
+++ b/tweet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Data Collection Time</t>
   </si>
@@ -35,34 +35,13 @@
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>2020-07-19 19:58:25.023965</t>
-  </si>
-  <si>
-    <t>Sun Jul 19 16:58:18 +0000 2020</t>
-  </si>
-  <si>
-    <t>@FatmaZehraDulg1</t>
-  </si>
-  <si>
-    <t>İstanbul, Türkiye</t>
-  </si>
-  <si>
-    <t>RT @cengizozakinci: ABD'nin Hitler'i Rusya'ya saldırtması; Rusya'yı Afganistan işgaline kışkırtması; Saddam'a Kuveyt işgali için yeşil ışık…</t>
-  </si>
-  <si>
-    <t>ABD'nin Hitler'i Rusya'ya saldırtması; Rusya'yı Afganistan işgaline kışkırtması; Saddam'a Kuveyt işgali için yeşil ışık yakması nasıl bu ülkeleri çökerten birer tuzak idiyse, Türkiye'yi 74 yıldır "İslam ülkelerinin lideri"(!) olmaya özendirmesi de yine bu türden bir tuzaktır.</t>
-  </si>
-  <si>
-    <t>https://t.co/6V2uW1yPvj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +56,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,20 +75,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,13 +375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,33 +404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>